<commit_message>
Updated the NewCustomerTest Page
</commit_message>
<xml_diff>
--- a/src/main/java/com/G99Bank/qa/testdata/newcsttestdata.xlsx
+++ b/src/main/java/com/G99Bank/qa/testdata/newcsttestdata.xlsx
@@ -185,7 +185,7 @@
     <t xml:space="preserve">9080706050</t>
   </si>
   <si>
-    <t xml:space="preserve">pavan.sisodia@test.com</t>
+    <t xml:space="preserve">pavan.s@test01.com</t>
   </si>
   <si>
     <t xml:space="preserve">pavan123</t>
@@ -203,7 +203,7 @@
     <t xml:space="preserve">9988776655</t>
   </si>
   <si>
-    <t xml:space="preserve">babu.shekhawat@test.com</t>
+    <t xml:space="preserve">babu.s@test01.com</t>
   </si>
   <si>
     <t xml:space="preserve">babu123</t>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">7778886661</t>
   </si>
   <si>
-    <t xml:space="preserve">jagan.singh@test.com</t>
+    <t xml:space="preserve">jagan.s@test01.com</t>
   </si>
   <si>
     <t xml:space="preserve">jagan123</t>
@@ -239,7 +239,7 @@
     <t xml:space="preserve">7689051234</t>
   </si>
   <si>
-    <t xml:space="preserve">roja.agarwal@test.com</t>
+    <t xml:space="preserve">roja.a@test01.com</t>
   </si>
   <si>
     <t xml:space="preserve">roja123</t>
@@ -696,7 +696,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -870,10 +870,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="pavan.sisodia@test.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="babu.shekhawat@test.com"/>
-    <hyperlink ref="I4" r:id="rId3" display="jagan.singh@test.com"/>
-    <hyperlink ref="I5" r:id="rId4" display="roja.agarwal@test.com"/>
+    <hyperlink ref="I2" r:id="rId1" display="pavan.s@test01.com"/>
+    <hyperlink ref="I3" r:id="rId2" display="babu.s@test01.com"/>
+    <hyperlink ref="I4" r:id="rId3" display="jagan.s@test01.com"/>
+    <hyperlink ref="I5" r:id="rId4" display="roja.a@test01.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>